<commit_message>
updating summary and adding proof outline for squares
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zachhansen/Desktop/anthem-benchmarks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20863B2-2855-564A-952C-64923CDDEEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BF8ECB-44FB-DE45-BF19-3DFE2BCF29D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{B95AA593-8B88-5A46-A9C4-59DB3E682607}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B95AA593-8B88-5A46-A9C4-59DB3E682607}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="56">
   <si>
     <t>Equivalence</t>
   </si>
@@ -122,9 +122,6 @@
     <t>trivial_primes</t>
   </si>
   <si>
-    <t>Runtime (ms)</t>
-  </si>
-  <si>
     <t>lin2</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>X = 0..1</t>
-  </si>
-  <si>
     <t>X = 0..3</t>
   </si>
   <si>
@@ -185,26 +179,38 @@
     <t>optimized_primes</t>
   </si>
   <si>
-    <t>No eq-break Runtime</t>
-  </si>
-  <si>
     <t>Needs proof outline</t>
   </si>
   <si>
-    <t>Suspected to be SE</t>
-  </si>
-  <si>
     <t>Problem</t>
   </si>
   <si>
     <t>Backwards only (incomplete specification of division), needs PO</t>
+  </si>
+  <si>
+    <t>Suspected to be SE (experimental)</t>
+  </si>
+  <si>
+    <t>This is the external equivalence variation of squares, where the bound is a placeholder.</t>
+  </si>
+  <si>
+    <t>This problem is interesting. Providing a lemma "n*n = (-n)*(-n)" makes it trivial.</t>
+  </si>
+  <si>
+    <t>But, Anthem doesn’t support proof outlines for testing strong equivalence yet.</t>
+  </si>
+  <si>
+    <t>Runtime with eq-break (ms)</t>
+  </si>
+  <si>
+    <t>No eq-break Runtime (ms)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -218,6 +224,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -240,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <extLst>
@@ -250,6 +262,7 @@
       </extLst>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52310458-30C4-ED4F-A140-FBA28E5C016D}">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="136" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="136" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -612,15 +625,15 @@
     <col min="1" max="1" width="28.1640625" customWidth="1"/>
     <col min="3" max="3" width="14.1640625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" customWidth="1"/>
-    <col min="10" max="10" width="25.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.5" customWidth="1"/>
+    <col min="8" max="8" width="24.5" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" customWidth="1"/>
+    <col min="10" max="10" width="85.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -635,19 +648,19 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>40</v>
-      </c>
       <c r="J1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -666,17 +679,17 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2">
+        <v>10503</v>
+      </c>
+      <c r="H2">
         <v>10502</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2">
-        <v>10503</v>
+      <c r="I2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -695,17 +708,17 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3">
+        <v>1661</v>
+      </c>
+      <c r="H3">
         <v>1648</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3">
-        <v>1661</v>
+      <c r="I3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -724,17 +737,17 @@
       <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4">
+        <v>23</v>
+      </c>
+      <c r="H4">
         <v>21</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4">
-        <v>23</v>
+      <c r="I4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -753,17 +766,17 @@
       <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5">
         <v>21</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5">
+      <c r="H5">
         <v>21</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -782,17 +795,17 @@
       <c r="E6" t="s">
         <v>7</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6">
+        <v>25</v>
+      </c>
+      <c r="H6">
         <v>27</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6">
-        <v>25</v>
+      <c r="I6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -811,17 +824,17 @@
       <c r="E7" t="s">
         <v>7</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7">
+        <v>141</v>
+      </c>
+      <c r="H7">
         <v>129</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7">
-        <v>141</v>
+      <c r="I7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -840,17 +853,17 @@
       <c r="E8" t="s">
         <v>7</v>
       </c>
-      <c r="F8">
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8">
+        <v>52</v>
+      </c>
+      <c r="H8">
         <v>46</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8">
-        <v>52</v>
+      <c r="I8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -869,17 +882,17 @@
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F9">
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9">
+        <v>48</v>
+      </c>
+      <c r="H9">
         <v>46</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9">
-        <v>48</v>
+      <c r="I9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -898,17 +911,17 @@
       <c r="E10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F10">
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10">
+        <v>11</v>
+      </c>
+      <c r="H10">
         <v>13</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10">
-        <v>11</v>
+      <c r="I10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -927,17 +940,17 @@
       <c r="E11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F11">
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11">
+        <v>12</v>
+      </c>
+      <c r="H11">
         <v>11</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11">
-        <v>12</v>
+      <c r="I11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -956,20 +969,20 @@
       <c r="E12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12">
-        <v>5</v>
-      </c>
-      <c r="H12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" t="s">
-        <v>51</v>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12">
+        <v>5</v>
       </c>
       <c r="J12" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -988,20 +1001,20 @@
       <c r="E13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13">
-        <v>5</v>
-      </c>
-      <c r="H13" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" t="s">
-        <v>51</v>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13">
+        <v>5</v>
       </c>
       <c r="J13" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -1020,17 +1033,17 @@
       <c r="E14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F14">
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14">
+        <v>72</v>
+      </c>
+      <c r="H14">
         <v>71</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14" t="s">
-        <v>22</v>
-      </c>
-      <c r="J14">
-        <v>72</v>
+      <c r="I14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -1049,17 +1062,17 @@
       <c r="E15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F15">
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15">
+        <v>310</v>
+      </c>
+      <c r="H15">
         <v>302</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15" t="s">
-        <v>22</v>
-      </c>
-      <c r="J15">
-        <v>310</v>
+      <c r="I15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -1078,17 +1091,17 @@
       <c r="E16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F16">
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16">
+        <v>75</v>
+      </c>
+      <c r="H16">
         <v>68</v>
       </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16">
-        <v>75</v>
+      <c r="I16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -1107,22 +1120,22 @@
       <c r="E17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F17">
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17">
+        <v>6231</v>
+      </c>
+      <c r="H17">
         <v>11220</v>
       </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
-        <v>22</v>
-      </c>
-      <c r="J17">
-        <v>6231</v>
+      <c r="I17">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
@@ -1136,22 +1149,22 @@
       <c r="E18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F18">
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18">
         <v>30</v>
       </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
-        <v>22</v>
-      </c>
-      <c r="J18">
+      <c r="H18">
         <v>30</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
@@ -1165,22 +1178,22 @@
       <c r="E19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F19">
-        <v>29</v>
+      <c r="F19" t="s">
+        <v>22</v>
       </c>
       <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19" t="s">
-        <v>22</v>
-      </c>
-      <c r="J19">
-        <v>29</v>
+        <v>29</v>
+      </c>
+      <c r="H19">
+        <v>29</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
@@ -1194,25 +1207,25 @@
       <c r="E20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F20">
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20">
+        <v>77</v>
+      </c>
+      <c r="H20">
         <v>68</v>
       </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I20" t="s">
-        <v>41</v>
-      </c>
-      <c r="J20">
-        <v>77</v>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
@@ -1226,25 +1239,25 @@
       <c r="E21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F21">
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21">
+        <v>638</v>
+      </c>
+      <c r="H21">
         <v>668</v>
       </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21" t="s">
-        <v>22</v>
-      </c>
-      <c r="I21" t="s">
-        <v>41</v>
-      </c>
-      <c r="J21">
-        <v>638</v>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
@@ -1258,25 +1271,25 @@
       <c r="E22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F22">
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22">
+        <v>2050</v>
+      </c>
+      <c r="H22">
         <v>2027</v>
       </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22" t="s">
-        <v>22</v>
-      </c>
-      <c r="I22" t="s">
-        <v>42</v>
-      </c>
-      <c r="J22">
-        <v>2050</v>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -1290,25 +1303,25 @@
       <c r="E23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23">
-        <v>5</v>
-      </c>
-      <c r="H23" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" t="s">
-        <v>42</v>
+      <c r="F23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23">
+        <v>5</v>
       </c>
       <c r="J23" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
@@ -1322,25 +1335,25 @@
       <c r="E24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F24">
+      <c r="F24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" t="s">
+        <v>35</v>
+      </c>
+      <c r="H24">
         <v>20922</v>
       </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="H24" t="s">
-        <v>22</v>
-      </c>
-      <c r="I24" t="s">
-        <v>43</v>
+      <c r="I24">
+        <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
@@ -1354,25 +1367,25 @@
       <c r="E25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G25">
-        <v>5</v>
-      </c>
-      <c r="H25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" t="s">
-        <v>43</v>
+      <c r="F25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25">
+        <v>5</v>
       </c>
       <c r="J25" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -1386,25 +1399,25 @@
       <c r="E26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G26">
-        <v>5</v>
-      </c>
-      <c r="H26" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J26" t="s">
-        <v>30</v>
+      <c r="F26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" t="s">
+        <v>29</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I26">
+        <v>5</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
@@ -1418,25 +1431,25 @@
       <c r="E27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>36</v>
+      <c r="F27" t="s">
+        <v>22</v>
       </c>
       <c r="G27" t="s">
-        <v>36</v>
-      </c>
-      <c r="H27" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J27" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I27">
+        <v>5</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
         <v>5</v>
@@ -1450,25 +1463,25 @@
       <c r="E28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G28">
-        <v>5</v>
-      </c>
-      <c r="H28" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J28" t="s">
-        <v>36</v>
+      <c r="F28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I28">
+        <v>5</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
@@ -1483,19 +1496,19 @@
         <v>7</v>
       </c>
       <c r="F29" t="s">
-        <v>30</v>
-      </c>
-      <c r="G29">
-        <v>5</v>
+        <v>22</v>
+      </c>
+      <c r="G29" t="s">
+        <v>35</v>
       </c>
       <c r="H29" t="s">
-        <v>22</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J29" t="s">
-        <v>36</v>
+        <v>29</v>
+      </c>
+      <c r="I29">
+        <v>5</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -1514,17 +1527,17 @@
       <c r="E30" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F30">
+      <c r="F30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30">
+        <v>114</v>
+      </c>
+      <c r="H30">
         <v>102</v>
       </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30" t="s">
-        <v>22</v>
-      </c>
-      <c r="J30">
-        <v>114</v>
+      <c r="I30">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -1543,17 +1556,17 @@
       <c r="E31" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F31">
+      <c r="F31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31">
+        <v>92</v>
+      </c>
+      <c r="H31">
         <v>100</v>
       </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31" t="s">
-        <v>22</v>
-      </c>
-      <c r="J31">
-        <v>92</v>
+      <c r="I31">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -1572,17 +1585,17 @@
       <c r="E32" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F32">
+      <c r="F32" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32">
+        <v>71</v>
+      </c>
+      <c r="H32">
         <v>96</v>
       </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32" t="s">
-        <v>22</v>
-      </c>
-      <c r="J32">
-        <v>71</v>
+      <c r="I32">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -1601,17 +1614,17 @@
       <c r="E33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F33">
+      <c r="F33" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33">
+        <v>74</v>
+      </c>
+      <c r="H33">
         <v>96</v>
       </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33" t="s">
-        <v>22</v>
-      </c>
-      <c r="J33">
-        <v>74</v>
+      <c r="I33">
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -1630,17 +1643,17 @@
       <c r="E34" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F34">
+      <c r="F34" t="s">
+        <v>22</v>
+      </c>
+      <c r="G34">
+        <v>68</v>
+      </c>
+      <c r="H34">
         <v>100</v>
       </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34" t="s">
-        <v>22</v>
-      </c>
-      <c r="J34">
-        <v>68</v>
+      <c r="I34">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -1659,22 +1672,22 @@
       <c r="E35" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F35">
+      <c r="F35" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35">
+        <v>78</v>
+      </c>
+      <c r="H35">
         <v>83</v>
       </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35" t="s">
-        <v>22</v>
-      </c>
-      <c r="J35">
-        <v>78</v>
+      <c r="I35">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
         <v>13</v>
@@ -1688,25 +1701,25 @@
       <c r="E36" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H36" t="s">
-        <v>22</v>
-      </c>
-      <c r="I36" t="s">
-        <v>53</v>
+      <c r="F36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" t="s">
+        <v>29</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="J36" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
         <v>13</v>
@@ -1720,20 +1733,20 @@
       <c r="E37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H37" t="s">
-        <v>22</v>
-      </c>
-      <c r="I37" t="s">
-        <v>53</v>
+      <c r="F37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G37" t="s">
+        <v>29</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="J37" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -1752,20 +1765,20 @@
       <c r="E38" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H38" t="s">
-        <v>22</v>
-      </c>
-      <c r="I38" t="s">
-        <v>39</v>
+      <c r="F38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G38" t="s">
+        <v>35</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I38" s="1">
+        <v>5</v>
       </c>
       <c r="J38" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -1784,20 +1797,20 @@
       <c r="E39" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H39" t="s">
-        <v>22</v>
-      </c>
-      <c r="I39" t="s">
-        <v>39</v>
+      <c r="F39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39" t="s">
+        <v>35</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I39" s="1">
+        <v>5</v>
       </c>
       <c r="J39" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
@@ -1816,17 +1829,17 @@
       <c r="E40" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F40">
+      <c r="F40" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" t="s">
+        <v>29</v>
+      </c>
+      <c r="H40">
         <v>22712</v>
       </c>
-      <c r="G40">
+      <c r="I40">
         <v>3</v>
-      </c>
-      <c r="H40" t="s">
-        <v>22</v>
-      </c>
-      <c r="J40" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
@@ -1845,17 +1858,17 @@
       <c r="E41" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G41">
-        <v>5</v>
-      </c>
-      <c r="H41" t="s">
-        <v>22</v>
-      </c>
-      <c r="J41" t="s">
-        <v>30</v>
+      <c r="F41" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" t="s">
+        <v>29</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I41">
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -1874,20 +1887,20 @@
       <c r="E42" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F42">
+      <c r="F42" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H42">
         <v>24267</v>
       </c>
-      <c r="G42">
+      <c r="I42">
         <v>3</v>
       </c>
-      <c r="H42" t="s">
-        <v>22</v>
-      </c>
-      <c r="I42" t="s">
-        <v>50</v>
-      </c>
       <c r="J42" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
@@ -1906,20 +1919,20 @@
       <c r="E43" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G43">
-        <v>5</v>
-      </c>
-      <c r="H43" t="s">
-        <v>22</v>
-      </c>
-      <c r="I43" t="s">
-        <v>50</v>
+      <c r="F43" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" t="s">
+        <v>29</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I43">
+        <v>5</v>
       </c>
       <c r="J43" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
@@ -1938,17 +1951,17 @@
       <c r="E44" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G44">
-        <v>5</v>
-      </c>
-      <c r="H44" t="s">
-        <v>22</v>
-      </c>
-      <c r="J44" t="s">
-        <v>36</v>
+      <c r="F44" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" t="s">
+        <v>35</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I44">
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
@@ -1967,17 +1980,17 @@
       <c r="E45" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G45">
-        <v>5</v>
-      </c>
-      <c r="H45" t="s">
-        <v>22</v>
-      </c>
-      <c r="J45" t="s">
-        <v>36</v>
+      <c r="F45" t="s">
+        <v>22</v>
+      </c>
+      <c r="G45" t="s">
+        <v>35</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I45">
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
@@ -1996,17 +2009,20 @@
       <c r="E46" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>30</v>
+      <c r="F46" t="s">
+        <v>22</v>
       </c>
       <c r="G46">
-        <v>5</v>
-      </c>
-      <c r="H46" t="s">
-        <v>22</v>
+        <v>252</v>
+      </c>
+      <c r="H46" s="1">
+        <v>396</v>
+      </c>
+      <c r="I46">
+        <v>3</v>
       </c>
       <c r="J46" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
@@ -2025,22 +2041,25 @@
       <c r="E47" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G47">
-        <v>5</v>
-      </c>
-      <c r="H47" t="s">
-        <v>22</v>
+      <c r="F47" t="s">
+        <v>22</v>
+      </c>
+      <c r="G47" t="s">
+        <v>29</v>
+      </c>
+      <c r="H47" s="1">
+        <v>11283</v>
+      </c>
+      <c r="I47">
+        <v>3</v>
       </c>
       <c r="J47" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
         <v>13</v>
@@ -2054,22 +2073,22 @@
       <c r="E48" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F48">
+      <c r="F48" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48">
+        <v>5816</v>
+      </c>
+      <c r="H48">
         <v>4905</v>
       </c>
-      <c r="G48">
-        <v>1</v>
-      </c>
-      <c r="H48" t="s">
-        <v>22</v>
-      </c>
-      <c r="J48">
-        <v>5816</v>
+      <c r="I48">
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B49" t="s">
         <v>13</v>
@@ -2083,22 +2102,22 @@
       <c r="E49" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F49">
+      <c r="F49" t="s">
+        <v>22</v>
+      </c>
+      <c r="G49" t="s">
+        <v>29</v>
+      </c>
+      <c r="H49">
         <v>16879</v>
       </c>
-      <c r="G49">
-        <v>1</v>
-      </c>
-      <c r="H49" t="s">
-        <v>22</v>
-      </c>
-      <c r="J49" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="20" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B50" t="s">
         <v>13</v>
@@ -2112,22 +2131,23 @@
       <c r="E50" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>30</v>
+      <c r="F50" t="s">
+        <v>22</v>
       </c>
       <c r="G50">
-        <v>5</v>
-      </c>
-      <c r="H50" t="s">
-        <v>22</v>
-      </c>
-      <c r="I50" t="s">
-        <v>50</v>
-      </c>
+        <v>316094</v>
+      </c>
+      <c r="H50" s="1">
+        <v>324012</v>
+      </c>
+      <c r="I50">
+        <v>4</v>
+      </c>
+      <c r="J50" s="3"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B51" t="s">
         <v>13</v>
@@ -2141,17 +2161,17 @@
       <c r="E51" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G51">
-        <v>5</v>
-      </c>
-      <c r="H51" t="s">
-        <v>22</v>
-      </c>
-      <c r="I51" t="s">
-        <v>50</v>
+      <c r="F51" t="s">
+        <v>22</v>
+      </c>
+      <c r="G51" t="s">
+        <v>35</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
@@ -2170,8 +2190,8 @@
       <c r="E53" t="s">
         <v>14</v>
       </c>
-      <c r="H53" t="s">
-        <v>37</v>
+      <c r="F53" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
@@ -2190,8 +2210,8 @@
       <c r="E54" t="s">
         <v>14</v>
       </c>
-      <c r="H54" t="s">
-        <v>37</v>
+      <c r="F54" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
@@ -2210,8 +2230,8 @@
       <c r="E55" t="s">
         <v>14</v>
       </c>
-      <c r="H55" t="s">
-        <v>37</v>
+      <c r="F55" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
@@ -2230,13 +2250,13 @@
       <c r="E56" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H56" t="s">
-        <v>37</v>
+      <c r="F56" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B57" t="s">
         <v>5</v>
@@ -2250,13 +2270,13 @@
       <c r="E57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H57" t="s">
-        <v>37</v>
+      <c r="F57" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B58" t="s">
         <v>5</v>
@@ -2270,8 +2290,8 @@
       <c r="E58" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H58" t="s">
-        <v>37</v>
+      <c r="F58" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
@@ -2288,10 +2308,10 @@
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>46</v>
-      </c>
-      <c r="H59" t="s">
-        <v>37</v>
+        <v>44</v>
+      </c>
+      <c r="F59" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
@@ -2308,10 +2328,10 @@
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>46</v>
-      </c>
-      <c r="H60" t="s">
-        <v>37</v>
+        <v>44</v>
+      </c>
+      <c r="F60" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
@@ -2328,10 +2348,10 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>46</v>
-      </c>
-      <c r="H61" t="s">
-        <v>37</v>
+        <v>44</v>
+      </c>
+      <c r="F61" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
@@ -2348,10 +2368,10 @@
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>46</v>
-      </c>
-      <c r="H62" t="s">
-        <v>37</v>
+        <v>44</v>
+      </c>
+      <c r="F62" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
@@ -2368,10 +2388,10 @@
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>46</v>
-      </c>
-      <c r="H63" t="s">
-        <v>37</v>
+        <v>44</v>
+      </c>
+      <c r="F63" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
@@ -2388,13 +2408,13 @@
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>46</v>
-      </c>
-      <c r="H64" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="F64" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>25</v>
       </c>
@@ -2408,13 +2428,13 @@
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>46</v>
-      </c>
-      <c r="H65" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="F65" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>25</v>
       </c>
@@ -2428,13 +2448,13 @@
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>46</v>
-      </c>
-      <c r="H66" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="F66" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>26</v>
       </c>
@@ -2448,13 +2468,13 @@
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>46</v>
-      </c>
-      <c r="H67" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="F67" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>26</v>
       </c>
@@ -2468,13 +2488,13 @@
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>46</v>
-      </c>
-      <c r="H68" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="F68" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>27</v>
       </c>
@@ -2488,13 +2508,13 @@
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>46</v>
-      </c>
-      <c r="H69" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="F69" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>27</v>
       </c>
@@ -2508,15 +2528,15 @@
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>46</v>
-      </c>
-      <c r="H70" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="F70" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B71" t="s">
         <v>5</v>
@@ -2528,15 +2548,15 @@
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>46</v>
-      </c>
-      <c r="H71" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="F71" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B72" t="s">
         <v>5</v>
@@ -2548,10 +2568,10 @@
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>46</v>
-      </c>
-      <c r="H72" t="s">
-        <v>37</v>
+        <v>44</v>
+      </c>
+      <c r="F72" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>